<commit_message>
Updated comments, Readme and Individual Assessment file
</commit_message>
<xml_diff>
--- a/Documents/Individual Assessment.xlsx
+++ b/Documents/Individual Assessment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karld\IdeaProjects\group-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karld\IdeaProjects\group-project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E500090-83C0-40F3-9993-B34FD3A10162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AFC461-6FFA-4F7A-BECF-760DFB02AD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1845" yWindow="4500" windowWidth="28785" windowHeight="15345" xr2:uid="{E82A4A5C-E753-4B05-8D34-C0B8E80B2BF5}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +470,9 @@
       <c r="B2" s="4">
         <v>25</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4">
+        <v>25</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -482,7 +484,9 @@
       <c r="B3" s="4">
         <v>25</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4">
+        <v>25</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -494,7 +498,9 @@
       <c r="B4" s="4">
         <v>25</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4">
+        <v>25</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -506,7 +512,9 @@
       <c r="B5" s="4">
         <v>25</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>25</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>

</xml_diff>